<commit_message>
Feat/49/transfer crud (#51) (#52)
* feat: Transferドメイン作成

* feat: Transfer/CRUDメソッド列挙

* refactor: TransferMapper.xmlに統一

* feat: findOne,deleteはselectorを引数にする

* update: findOne,deleteはselectorを引数にすることに伴う変更

* refactor: クエリパラメータtransferId -> id

* feat: inset, set,delete追加(xml)

* refactor: parameterTypeの指定

* feat: repositoryImpl実装

* fix: set-> add

* test: TransferControllerTest実装

* test: TransferServiceImplTest実装

* test: TransferRepositoryImplTest実装

* feat: TemporaryTransfer, transferId追加

* test: テストデータにtransferテーブル追加

* test: テストデータにtransferテーブル追加に伴う修正

* fix: temporaryTransfer/transferId追加に伴う修正

* fix: sqlミス修正

* test: エクセル変更

* test: TemporaryTransfer/transferId追加に伴う変更

* feat: Transfer削除時,関連するTemporaryも削除

* test: Transfer削除時,関連するTemporaryも削除の変更に伴う修正

* test: TransferRepositoryImplDbUnitTest実装
</commit_message>
<xml_diff>
--- a/src/test/java/com/example/moneyAllocation/repository/data/account_delete_expected.xlsx
+++ b/src/test/java/com/example/moneyAllocation/repository/data/account_delete_expected.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryotasato/local-dev/MoneyAllocation/allocation-api/src/test/java/com/example/moneyAllocation/repository/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD04177B-5579-3147-96FD-A191E2F6D69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510F2135-A373-5944-91B9-7935118844C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22920" yWindow="14400" windowWidth="22920" windowHeight="14400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22200" yWindow="11660" windowWidth="22920" windowHeight="14400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="3" r:id="rId1"/>
     <sheet name="ACCOUNT" sheetId="2" r:id="rId2"/>
-    <sheet name="REGULAR_TRANSFER" sheetId="7" r:id="rId3"/>
-    <sheet name="TEMPORARY_TRANSFER" sheetId="5" r:id="rId4"/>
+    <sheet name="TRANSFER" sheetId="8" r:id="rId3"/>
+    <sheet name="REGULAR_TRANSFER" sheetId="7" r:id="rId4"/>
+    <sheet name="TEMPORARY_TRANSFER" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>三井</t>
   </si>
@@ -159,6 +160,26 @@
   </si>
   <si>
     <t>楽天</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2023/06</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2023/07</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2022/09</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TRANSFER_ID</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -207,11 +228,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1421,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D0E107-AE2E-2D42-AB9F-FAD47DEB0DE0}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1542,6 +1566,66 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6846CA1-B1C7-A24D-9C23-6AA1748C456E}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A80971-0ABB-7042-8F2B-8079DE03962B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -1652,17 +1736,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88235FF5-1F89-A44E-A56F-C79DCAC8D673}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="28">
+    <row r="1" spans="1:7" ht="28">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1681,8 +1765,11 @@
       <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="14">
+      <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1701,8 +1788,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="14">
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1721,8 +1811,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="14">
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1740,6 +1833,9 @@
       </c>
       <c r="F4" s="1">
         <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>